<commit_message>
Created Allocate Workout Screen, Implemented Delete and Update Workout Functionality
</commit_message>
<xml_diff>
--- a/Documents/Gnatt Chart.xlsx
+++ b/Documents/Gnatt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT-Digital-Systems-Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2AED15-86B9-42DE-8398-1A044A63513F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5D2AED15-86B9-42DE-8398-1A044A63513F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFDB9465-94DD-4958-B7EC-3D5240C46D73}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{4BFAF75B-F8AC-4376-A3AD-AF0EB7737F25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4BFAF75B-F8AC-4376-A3AD-AF0EB7737F25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,12 +278,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF797575"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,10 +427,21 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,18 +456,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506F536C-643D-47FA-A80F-5E0A5FE49105}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +799,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="28"/>
@@ -824,12 +817,12 @@
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
       <c r="L1" s="28"/>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="37"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="31"/>
       <c r="Q1" s="28" t="s">
         <v>4</v>
       </c>
@@ -853,7 +846,7 @@
       </c>
       <c r="AD1" s="28"/>
       <c r="AE1" s="28"/>
-      <c r="AF1" s="29"/>
+      <c r="AF1" s="32"/>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -961,7 +954,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="33" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="3"/>
@@ -975,7 +968,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="33" t="s">
+      <c r="T3" s="36" t="s">
         <v>14</v>
       </c>
       <c r="U3" s="1"/>
@@ -985,13 +978,13 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="31" t="s">
+      <c r="AB3" s="34" t="s">
         <v>15</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="32" t="s">
+      <c r="AF3" s="35" t="s">
         <v>12</v>
       </c>
       <c r="AI3" s="2"/>
@@ -1005,7 +998,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="30"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1017,7 +1010,7 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="20"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="33"/>
+      <c r="T4" s="36"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1025,11 +1018,11 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="31"/>
+      <c r="AB4" s="34"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="32"/>
+      <c r="AF4" s="35"/>
       <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
@@ -1040,7 +1033,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="30"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1052,7 +1045,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="33"/>
+      <c r="T5" s="36"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1060,11 +1053,11 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="31"/>
+      <c r="AB5" s="34"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="32"/>
+      <c r="AF5" s="35"/>
       <c r="AH5" s="11" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1073,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="30"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1092,7 +1085,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="33"/>
+      <c r="T6" s="36"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1100,11 +1093,11 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="31"/>
+      <c r="AB6" s="34"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="32"/>
+      <c r="AF6" s="35"/>
       <c r="AH6" s="22"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="12" t="s">
@@ -1119,7 +1112,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="30"/>
+      <c r="H7" s="33"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1131,7 +1124,7 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="33"/>
+      <c r="T7" s="36"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1139,11 +1132,11 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="31"/>
+      <c r="AB7" s="34"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
-      <c r="AF7" s="32"/>
+      <c r="AF7" s="35"/>
       <c r="AH7" s="23"/>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="12" t="s">
@@ -1158,7 +1151,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="30"/>
+      <c r="H8" s="33"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1170,7 +1163,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="33"/>
+      <c r="T8" s="36"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -1178,11 +1171,11 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
-      <c r="AB8" s="31"/>
+      <c r="AB8" s="34"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="32"/>
+      <c r="AF8" s="35"/>
       <c r="AH8" s="24"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="12" t="s">
@@ -1197,7 +1190,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="30"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1209,7 +1202,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="33"/>
+      <c r="T9" s="36"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -1217,11 +1210,11 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="31"/>
+      <c r="AB9" s="34"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
-      <c r="AF9" s="32"/>
+      <c r="AF9" s="35"/>
       <c r="AH9" s="25"/>
       <c r="AI9" s="15"/>
       <c r="AJ9" s="12" t="s">
@@ -1236,7 +1229,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="30"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1248,7 +1241,7 @@
       <c r="Q10" s="23"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-      <c r="T10" s="33"/>
+      <c r="T10" s="36"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
@@ -1256,11 +1249,11 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
-      <c r="AB10" s="31"/>
+      <c r="AB10" s="34"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="14"/>
       <c r="AE10" s="1"/>
-      <c r="AF10" s="32"/>
+      <c r="AF10" s="35"/>
       <c r="AH10" s="26"/>
       <c r="AI10" s="7"/>
       <c r="AJ10" s="12" t="s">
@@ -1275,7 +1268,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="30"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1287,7 +1280,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="33"/>
+      <c r="T11" s="36"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -1295,11 +1288,11 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="31"/>
+      <c r="AB11" s="34"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
-      <c r="AF11" s="32"/>
+      <c r="AF11" s="35"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -1309,7 +1302,7 @@
       <c r="E12" s="25"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="30"/>
+      <c r="H12" s="33"/>
       <c r="I12" s="20"/>
       <c r="J12" s="3"/>
       <c r="K12" s="20"/>
@@ -1321,19 +1314,19 @@
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
-      <c r="T12" s="33"/>
+      <c r="T12" s="36"/>
       <c r="U12" s="25"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="15"/>
-      <c r="AB12" s="31"/>
+      <c r="AB12" s="34"/>
       <c r="AC12" s="15"/>
       <c r="AD12" s="15"/>
       <c r="AE12" s="1"/>
-      <c r="AF12" s="32"/>
+      <c r="AF12" s="35"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1343,7 +1336,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="30"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1355,7 +1348,7 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="33"/>
+      <c r="T13" s="36"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -1363,11 +1356,11 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="31"/>
+      <c r="AB13" s="34"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="32"/>
+      <c r="AF13" s="35"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="11" t="s">
         <v>20</v>
@@ -1381,7 +1374,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="30"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1393,7 +1386,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="33"/>
+      <c r="T14" s="36"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
@@ -1401,11 +1394,11 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
-      <c r="AB14" s="31"/>
+      <c r="AB14" s="34"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
-      <c r="AF14" s="32"/>
+      <c r="AF14" s="35"/>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="12" t="s">
         <v>16</v>
@@ -1419,7 +1412,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="30"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1431,7 +1424,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="33"/>
+      <c r="T15" s="36"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -1439,11 +1432,11 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="31"/>
+      <c r="AB15" s="34"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
-      <c r="AF15" s="32"/>
+      <c r="AF15" s="35"/>
       <c r="AI15" s="20"/>
       <c r="AJ15" s="12" t="s">
         <v>23</v>
@@ -1457,7 +1450,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="30"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1469,7 +1462,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
-      <c r="T16" s="33"/>
+      <c r="T16" s="36"/>
       <c r="U16" s="13"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -1477,11 +1470,11 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
-      <c r="AB16" s="31"/>
+      <c r="AB16" s="34"/>
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
       <c r="AE16" s="13"/>
-      <c r="AF16" s="32"/>
+      <c r="AF16" s="35"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1491,7 +1484,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="30"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1503,7 +1496,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="33"/>
+      <c r="T17" s="36"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -1511,19 +1504,14 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="31"/>
+      <c r="AB17" s="34"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
-      <c r="AF17" s="32"/>
+      <c r="AF17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="U1:X1"/>
@@ -1531,6 +1519,11 @@
     <mergeCell ref="AB3:AB17"/>
     <mergeCell ref="AF3:AF17"/>
     <mergeCell ref="T3:T17"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Reworked on Requirements and Design Chapters and added Sprint Table
</commit_message>
<xml_diff>
--- a/Documents/Gnatt Chart.xlsx
+++ b/Documents/Gnatt Chart.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{5D2AED15-86B9-42DE-8398-1A044A63513F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20453F33-FCA0-4A54-B71B-CC732A3D4968}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC72B2C-777B-426E-8F24-4CF96A7AC8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4BFAF75B-F8AC-4376-A3AD-AF0EB7737F25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4BFAF75B-F8AC-4376-A3AD-AF0EB7737F25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$AH$5:$AJ$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AF$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>September</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Implementing</t>
+  </si>
+  <si>
+    <t>Shipping Delay</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -378,11 +381,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -430,12 +470,27 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -445,20 +500,14 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,10 +537,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -793,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506F536C-643D-47FA-A80F-5E0A5FE49105}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5:AJ15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,54 +851,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="29" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="28" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28" t="s">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28" t="s">
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28" t="s">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="32"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="28"/>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -961,7 +1006,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="29" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="3"/>
@@ -975,7 +1020,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="32" t="s">
         <v>14</v>
       </c>
       <c r="U3" s="1"/>
@@ -985,13 +1030,13 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="34" t="s">
+      <c r="AB3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="31" t="s">
         <v>12</v>
       </c>
       <c r="AI3" s="2"/>
@@ -1005,7 +1050,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="33"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1017,7 +1062,7 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="20"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="36"/>
+      <c r="T4" s="32"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1025,11 +1070,11 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="34"/>
+      <c r="AB4" s="30"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="35"/>
+      <c r="AF4" s="31"/>
       <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
@@ -1040,7 +1085,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="33"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1052,7 +1097,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="36"/>
+      <c r="T5" s="32"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1060,11 +1105,11 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="34"/>
+      <c r="AB5" s="30"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="35"/>
+      <c r="AF5" s="31"/>
       <c r="AH5" s="11" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1125,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="33"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1092,7 +1137,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="36"/>
+      <c r="T6" s="32"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1100,11 +1145,11 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="34"/>
+      <c r="AB6" s="30"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="35"/>
+      <c r="AF6" s="31"/>
       <c r="AH6" s="22"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="12" t="s">
@@ -1119,7 +1164,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="33"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1131,7 +1176,7 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="36"/>
+      <c r="T7" s="32"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1139,11 +1184,11 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="34"/>
+      <c r="AB7" s="30"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
-      <c r="AF7" s="35"/>
+      <c r="AF7" s="31"/>
       <c r="AH7" s="23"/>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="12" t="s">
@@ -1158,7 +1203,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="33"/>
+      <c r="H8" s="29"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1170,7 +1215,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="36"/>
+      <c r="T8" s="32"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -1178,11 +1223,11 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="34"/>
+      <c r="AB8" s="30"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="35"/>
+      <c r="AF8" s="31"/>
       <c r="AH8" s="24"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="12" t="s">
@@ -1197,7 +1242,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="33"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1209,7 +1254,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="36"/>
+      <c r="T9" s="32"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -1217,11 +1262,11 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="34"/>
+      <c r="AB9" s="30"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
-      <c r="AF9" s="35"/>
+      <c r="AF9" s="31"/>
       <c r="AH9" s="25"/>
       <c r="AI9" s="15"/>
       <c r="AJ9" s="12" t="s">
@@ -1236,7 +1281,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="33"/>
+      <c r="H10" s="29"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1248,7 +1293,7 @@
       <c r="Q10" s="23"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-      <c r="T10" s="36"/>
+      <c r="T10" s="32"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
@@ -1256,11 +1301,11 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="34"/>
+      <c r="AB10" s="30"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="14"/>
       <c r="AE10" s="1"/>
-      <c r="AF10" s="35"/>
+      <c r="AF10" s="31"/>
       <c r="AH10" s="26"/>
       <c r="AI10" s="7"/>
       <c r="AJ10" s="12" t="s">
@@ -1275,7 +1320,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="33"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1287,7 +1332,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="36"/>
+      <c r="T11" s="32"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -1295,11 +1340,11 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="34"/>
+      <c r="AB11" s="30"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
-      <c r="AF11" s="35"/>
+      <c r="AF11" s="31"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -1309,19 +1354,21 @@
       <c r="E12" s="25"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="20"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="36"/>
+      <c r="P12" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="32"/>
       <c r="U12" s="25"/>
       <c r="V12" s="20"/>
       <c r="W12" s="20"/>
@@ -1329,11 +1376,11 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
       <c r="AA12" s="15"/>
-      <c r="AB12" s="34"/>
+      <c r="AB12" s="30"/>
       <c r="AC12" s="15"/>
       <c r="AD12" s="15"/>
       <c r="AE12" s="1"/>
-      <c r="AF12" s="35"/>
+      <c r="AF12" s="31"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1343,7 +1390,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="33"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1355,7 +1402,7 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="36"/>
+      <c r="T13" s="32"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -1363,11 +1410,11 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="34"/>
+      <c r="AB13" s="30"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="35"/>
+      <c r="AF13" s="31"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="11" t="s">
         <v>20</v>
@@ -1381,7 +1428,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="33"/>
+      <c r="H14" s="29"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1393,7 +1440,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="36"/>
+      <c r="T14" s="32"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
@@ -1401,11 +1448,11 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
-      <c r="AB14" s="34"/>
+      <c r="AB14" s="30"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
-      <c r="AF14" s="35"/>
+      <c r="AF14" s="31"/>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="12" t="s">
         <v>16</v>
@@ -1419,7 +1466,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="33"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1431,7 +1478,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="36"/>
+      <c r="T15" s="32"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -1439,11 +1486,11 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="34"/>
+      <c r="AB15" s="30"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
-      <c r="AF15" s="35"/>
+      <c r="AF15" s="31"/>
       <c r="AI15" s="20"/>
       <c r="AJ15" s="12" t="s">
         <v>23</v>
@@ -1457,7 +1504,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="33"/>
+      <c r="H16" s="29"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1469,19 +1516,19 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="13"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="20"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Y16" s="21"/>
+      <c r="Y16" s="3"/>
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
-      <c r="AB16" s="34"/>
+      <c r="AB16" s="30"/>
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
       <c r="AE16" s="13"/>
-      <c r="AF16" s="35"/>
+      <c r="AF16" s="31"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1491,7 +1538,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="33"/>
+      <c r="H17" s="29"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1503,7 +1550,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="36"/>
+      <c r="T17" s="32"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -1511,14 +1558,19 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="34"/>
+      <c r="AB17" s="30"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
-      <c r="AF17" s="35"/>
+      <c r="AF17" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="U1:X1"/>
@@ -1526,11 +1578,7 @@
     <mergeCell ref="AB3:AB17"/>
     <mergeCell ref="AF3:AF17"/>
     <mergeCell ref="T3:T17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="P12:S12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Sprint Log and Test Sheet
</commit_message>
<xml_diff>
--- a/Documents/Gnatt Chart.xlsx
+++ b/Documents/Gnatt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC72B2C-777B-426E-8F24-4CF96A7AC8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789924EB-5B16-474E-891A-947207F418B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4BFAF75B-F8AC-4376-A3AD-AF0EB7737F25}"/>
+    <workbookView xWindow="-27285" yWindow="2085" windowWidth="23010" windowHeight="12480" xr2:uid="{4BFAF75B-F8AC-4376-A3AD-AF0EB7737F25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -470,9 +470,21 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,18 +500,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,6 +507,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -838,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506F536C-643D-47FA-A80F-5E0A5FE49105}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12:Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,54 +860,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="34" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="27" t="s">
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27" t="s">
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27" t="s">
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="32"/>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -1006,7 +1015,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="33" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="3"/>
@@ -1020,7 +1029,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="32" t="s">
+      <c r="T3" s="36" t="s">
         <v>14</v>
       </c>
       <c r="U3" s="1"/>
@@ -1030,13 +1039,13 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="30" t="s">
+      <c r="AB3" s="34" t="s">
         <v>15</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="31" t="s">
+      <c r="AF3" s="35" t="s">
         <v>12</v>
       </c>
       <c r="AI3" s="2"/>
@@ -1050,7 +1059,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="29"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1062,7 +1071,7 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="20"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="32"/>
+      <c r="T4" s="36"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1070,11 +1079,11 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="30"/>
+      <c r="AB4" s="34"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="31"/>
+      <c r="AF4" s="35"/>
       <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
@@ -1085,7 +1094,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="29"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1097,7 +1106,7 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="32"/>
+      <c r="T5" s="36"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1105,11 +1114,11 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="30"/>
+      <c r="AB5" s="34"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="31"/>
+      <c r="AF5" s="35"/>
       <c r="AH5" s="11" t="s">
         <v>24</v>
       </c>
@@ -1125,7 +1134,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="29"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1137,7 +1146,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="32"/>
+      <c r="T6" s="36"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1145,11 +1154,11 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="30"/>
+      <c r="AB6" s="34"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
-      <c r="AF6" s="31"/>
+      <c r="AF6" s="35"/>
       <c r="AH6" s="22"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="12" t="s">
@@ -1164,7 +1173,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="29"/>
+      <c r="H7" s="33"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1176,7 +1185,7 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="32"/>
+      <c r="T7" s="36"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1184,11 +1193,11 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="30"/>
+      <c r="AB7" s="34"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
-      <c r="AF7" s="31"/>
+      <c r="AF7" s="35"/>
       <c r="AH7" s="23"/>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="12" t="s">
@@ -1203,7 +1212,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="29"/>
+      <c r="H8" s="33"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1215,7 +1224,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="32"/>
+      <c r="T8" s="36"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -1223,11 +1232,11 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="30"/>
+      <c r="AB8" s="34"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="31"/>
+      <c r="AF8" s="35"/>
       <c r="AH8" s="24"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="12" t="s">
@@ -1242,7 +1251,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="29"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1254,7 +1263,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="32"/>
+      <c r="T9" s="36"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -1262,11 +1271,11 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="30"/>
+      <c r="AB9" s="34"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
-      <c r="AF9" s="31"/>
+      <c r="AF9" s="35"/>
       <c r="AH9" s="25"/>
       <c r="AI9" s="15"/>
       <c r="AJ9" s="12" t="s">
@@ -1281,7 +1290,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="29"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1293,7 +1302,7 @@
       <c r="Q10" s="23"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-      <c r="T10" s="32"/>
+      <c r="T10" s="36"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
@@ -1301,11 +1310,11 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="30"/>
+      <c r="AB10" s="34"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="14"/>
       <c r="AE10" s="1"/>
-      <c r="AF10" s="31"/>
+      <c r="AF10" s="35"/>
       <c r="AH10" s="26"/>
       <c r="AI10" s="7"/>
       <c r="AJ10" s="12" t="s">
@@ -1320,7 +1329,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="29"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1332,7 +1341,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="32"/>
+      <c r="T11" s="36"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -1340,11 +1349,11 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="30"/>
+      <c r="AB11" s="34"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
-      <c r="AF11" s="31"/>
+      <c r="AF11" s="35"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -1354,7 +1363,7 @@
       <c r="E12" s="25"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="29"/>
+      <c r="H12" s="33"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="25"/>
@@ -1368,19 +1377,19 @@
       <c r="Q12" s="38"/>
       <c r="R12" s="38"/>
       <c r="S12" s="39"/>
-      <c r="T12" s="32"/>
+      <c r="T12" s="36"/>
       <c r="U12" s="25"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="42"/>
       <c r="AA12" s="15"/>
-      <c r="AB12" s="30"/>
+      <c r="AB12" s="34"/>
       <c r="AC12" s="15"/>
       <c r="AD12" s="15"/>
       <c r="AE12" s="1"/>
-      <c r="AF12" s="31"/>
+      <c r="AF12" s="35"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1390,7 +1399,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="29"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1402,7 +1411,7 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="32"/>
+      <c r="T13" s="36"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -1410,11 +1419,11 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="30"/>
+      <c r="AB13" s="34"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="31"/>
+      <c r="AF13" s="35"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="11" t="s">
         <v>20</v>
@@ -1428,7 +1437,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="29"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1440,7 +1449,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="32"/>
+      <c r="T14" s="36"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
@@ -1448,11 +1457,11 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
-      <c r="AB14" s="30"/>
+      <c r="AB14" s="34"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
-      <c r="AF14" s="31"/>
+      <c r="AF14" s="35"/>
       <c r="AI14" s="9"/>
       <c r="AJ14" s="12" t="s">
         <v>16</v>
@@ -1466,7 +1475,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="29"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1478,7 +1487,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="32"/>
+      <c r="T15" s="36"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -1486,11 +1495,11 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="30"/>
+      <c r="AB15" s="34"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
-      <c r="AF15" s="31"/>
+      <c r="AF15" s="35"/>
       <c r="AI15" s="20"/>
       <c r="AJ15" s="12" t="s">
         <v>23</v>
@@ -1504,7 +1513,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -1516,7 +1525,7 @@
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13"/>
-      <c r="T16" s="32"/>
+      <c r="T16" s="36"/>
       <c r="U16" s="20"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -1524,11 +1533,11 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
-      <c r="AB16" s="30"/>
+      <c r="AB16" s="34"/>
       <c r="AC16" s="13"/>
       <c r="AD16" s="13"/>
       <c r="AE16" s="13"/>
-      <c r="AF16" s="31"/>
+      <c r="AF16" s="35"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1538,7 +1547,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="29"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1550,7 +1559,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="32"/>
+      <c r="T17" s="36"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -1558,19 +1567,14 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="30"/>
+      <c r="AB17" s="34"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
-      <c r="AF17" s="31"/>
+      <c r="AF17" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
+  <mergeCells count="14">
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AC1:AF1"/>
     <mergeCell ref="U1:X1"/>
@@ -1579,6 +1583,12 @@
     <mergeCell ref="AF3:AF17"/>
     <mergeCell ref="T3:T17"/>
     <mergeCell ref="P12:S12"/>
+    <mergeCell ref="V12:Z12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>